<commit_message>
Documentos y arreglos finales
</commit_message>
<xml_diff>
--- a/OpenCart 3/src/main/resources/Logs.xlsx
+++ b/OpenCart 3/src/main/resources/Logs.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fannygiraldo/Documents/Septimo/Electiva profesional/OpenCart 3/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fannygiraldo/Documents/Septimo/Electiva profesional/git/Tarea-Final-QA/OpenCart 3/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C4277B-9AF9-F249-AE74-87ECD59C0659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E13DF1-BC66-8247-8D10-FD2225315180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17340" activeTab="1" xr2:uid="{FCBC34B2-A818-F044-89C0-9A29738035EA}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30240" windowHeight="17340" activeTab="3" xr2:uid="{FCBC34B2-A818-F044-89C0-9A29738035EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>FirstName</t>
   </si>
@@ -149,33 +149,6 @@
     <t>Warning: E-Mail Address is already registered!</t>
   </si>
   <si>
-    <t xml:space="preserve">Miguel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arteaga </t>
-  </si>
-  <si>
-    <t>miguel.arteaga@testmail.com</t>
-  </si>
-  <si>
-    <t>3.241212323E9</t>
-  </si>
-  <si>
-    <t>Passw0rd3!</t>
-  </si>
-  <si>
-    <t>miguel5.arteaga@testmail.com</t>
-  </si>
-  <si>
-    <t>Samuel</t>
-  </si>
-  <si>
-    <t>Rua</t>
-  </si>
-  <si>
-    <t>Samueell.rua2@testmail.com</t>
-  </si>
-  <si>
     <t>SUCCESS</t>
   </si>
   <si>
@@ -192,12 +165,6 @@
   </si>
   <si>
     <t>FALLIDO</t>
-  </si>
-  <si>
-    <t>Warning: Your account has exceeded allowed number of login attempts. Please try again in 1 hour.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>fake2.user@testmail.com</t>
@@ -244,9 +211,6 @@
 ×</t>
   </si>
   <si>
-    <t>2025-12-01 02:57:21</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -256,20 +220,13 @@
     <t>1</t>
   </si>
   <si>
-    <t>2025-12-01 03:00:04</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>Producto no encontrado en el carrito</t>
+    <t>PasswordConfirm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -331,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -354,17 +311,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,14 +673,18 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.83203125"/>
-    <col min="4" max="4" customWidth="true" width="18.33203125"/>
-    <col min="7" max="7" customWidth="true" width="25.5"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
+    <col min="8" max="8" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -728,445 +703,182 @@
       <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s" s="0">
+      <c r="H4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" t="s" s="0">
+      <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="G5" t="s" s="0">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" t="s" s="0">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s" s="0">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="G6" t="s" s="0">
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="H6" t="s" s="0">
+      <c r="H6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s" s="0">
+      <c r="D7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s" s="0">
+      <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="F7" t="s" s="0">
+      <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="s" s="0">
+      <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="H7" t="s" s="0">
+      <c r="H7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H9" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="G10" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H10" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="G11" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H11" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G12" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H12" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="F13" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G13" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H13" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="G14" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H14" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="E15" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="F15" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="G15" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H15" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="E16" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="F16" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="G16" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="H16" t="s" s="0">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s" s="0">
-        <v>44</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="E17" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="F17" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="H17" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F30" s="3"/>
     </row>
   </sheetData>
@@ -1178,17 +890,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.0"/>
-    <col min="2" max="2" customWidth="true" width="14.6640625"/>
-    <col min="3" max="3" customWidth="true" width="18.0"/>
-    <col min="4" max="4" customWidth="true" width="12.5"/>
-    <col min="5" max="5" customWidth="true" width="11.5"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1209,139 +921,54 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s" s="0">
-        <v>46</v>
+      <c r="E2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>49</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>55</v>
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="4:4" x14ac:dyDescent="0.2">
@@ -1369,12 +996,14 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="25.83203125"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="6" max="6" width="51.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1397,64 +1026,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>59</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>66</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.2">
@@ -1482,16 +1091,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E90F313-D6C4-7947-A834-05F9A1484BBC}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="19.33203125"/>
-    <col min="3" max="3" customWidth="true" width="17.5"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1511,98 +1122,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="E2" t="s" s="0">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s" s="0">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>67</v>
-      </c>
-      <c r="B3" t="s" s="0">
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="E3" t="s" s="0">
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s" s="0">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>71</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>69</v>
+      <c r="E3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>